<commit_message>
readded color to status
</commit_message>
<xml_diff>
--- a/docs/deliverable 2/Getana_Deliverable_2_ProductBacklog.xlsx
+++ b/docs/deliverable 2/Getana_Deliverable_2_ProductBacklog.xlsx
@@ -363,7 +363,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -390,11 +390,8 @@
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -411,7 +408,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,12 +444,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
@@ -460,7 +461,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1210,7 +1210,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1272,7 +1272,7 @@
       <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="0" t="n">
@@ -1292,7 +1292,7 @@
       <c r="D9" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="0" t="n">
@@ -1312,7 +1312,7 @@
       <c r="D10" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -1332,7 +1332,7 @@
       <c r="D11" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="0" t="n">
@@ -1352,7 +1352,7 @@
       <c r="D12" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -1372,7 +1372,7 @@
       <c r="D13" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="0" t="n">

</xml_diff>